<commit_message>
Upando atualizações no LLD
</commit_message>
<xml_diff>
--- a/Documentação/ATA/ATAmodelo.xlsx
+++ b/Documentação/ATA/ATAmodelo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe0713f97eca5c34/Documentos/FACULDADE/É ESSA PASTA AQUI Ó/grupo-05-adsa-20201/Documentação/ATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE3B832B-E675-4B2E-8CAC-1D2BD9767B2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{60B4484A-0B15-47CE-89B7-BB145887A860}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FFAA5AFF-B378-424E-8472-67DDE50875E8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{16432F68-735D-4949-B8B5-CA40982BF5BE}"/>
   </bookViews>
@@ -78,47 +78,47 @@
     <t>VINÍCIUS DA SILVA CONCEIÇÃO</t>
   </si>
   <si>
+    <t>RESPONSÁVEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> INÍCIO</t>
+  </si>
+  <si>
+    <t>PAUTAS PARA A PRÓXIMA REUNIÃO</t>
+  </si>
+  <si>
+    <t>REUNIÃO DE EQUIPE</t>
+  </si>
+  <si>
+    <t>PRÓXIMA REUNIÃO</t>
+  </si>
+  <si>
+    <t>DATA E HORA</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>CANAL DISCORD - SUPERVISOR</t>
+  </si>
+  <si>
+    <t>ANOTAÇÕES</t>
+  </si>
+  <si>
     <t>dd/mm/aaaa</t>
   </si>
   <si>
-    <t>RESPONSÁVEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> INÍCIO</t>
-  </si>
-  <si>
-    <t>PAUTAS PARA A PRÓXIMA REUNIÃO</t>
-  </si>
-  <si>
-    <t>REUNIÃO DE EQUIPE</t>
-  </si>
-  <si>
-    <t>PRÓXIMA REUNIÃO</t>
-  </si>
-  <si>
-    <t>DATA E HORA</t>
+    <t>0h</t>
   </si>
   <si>
     <t>dd/mm/aaaa  -  0h até 0h</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>0h</t>
-  </si>
-  <si>
-    <t>CANAL DISCORD - SUPERVISOR</t>
-  </si>
-  <si>
-    <t>ANOTAÇÕES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +169,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -479,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -494,33 +501,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -543,21 +529,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -566,32 +573,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -968,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B6A8763-DEA1-422F-86C4-639973A5AD32}">
   <dimension ref="F2:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30:J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,322 +1007,322 @@
     <col min="7" max="7" width="52.42578125" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="G4" s="16"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="12"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="26"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="6:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="16"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="12"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="26"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="6:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="8" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="20"/>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="6:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F8" s="3"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="28"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="29"/>
     </row>
     <row r="9" spans="6:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="12" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="22" t="s">
+      <c r="J9" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="14" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="24"/>
+      <c r="J10" s="15"/>
     </row>
     <row r="11" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="14" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" s="24"/>
+        <v>20</v>
+      </c>
+      <c r="J11" s="15"/>
     </row>
     <row r="12" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="24" t="s">
-        <v>22</v>
+      <c r="J12" s="15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="14" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="24"/>
+        <v>20</v>
+      </c>
+      <c r="J13" s="15"/>
     </row>
     <row r="14" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="24"/>
+      <c r="J14" s="15"/>
     </row>
     <row r="15" spans="6:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G15" s="26"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="28"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="29"/>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="6:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G16" s="43" t="s">
+      <c r="G16" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="H16" s="39"/>
-      <c r="I16" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" s="44"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="45"/>
     </row>
     <row r="17" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G17" s="26"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="45"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="20"/>
     </row>
     <row r="18" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G18" s="26"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="45"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="20"/>
     </row>
     <row r="19" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G19" s="26"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="45"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G20" s="26"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="45"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="20"/>
     </row>
     <row r="21" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G21" s="26"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="45"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="20"/>
     </row>
     <row r="22" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G22" s="26"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="45"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="20"/>
     </row>
     <row r="23" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G23" s="26"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="28"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="29"/>
     </row>
     <row r="24" spans="7:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G24" s="33" t="s">
+      <c r="G24" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="33" t="s">
         <v>19</v>
-      </c>
-      <c r="H24" s="25" t="s">
-        <v>20</v>
       </c>
       <c r="I24" s="34"/>
       <c r="J24" s="35"/>
     </row>
     <row r="25" spans="7:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G25" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="I25" s="36"/>
-      <c r="J25" s="37"/>
+      <c r="G25" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="37"/>
+      <c r="J25" s="38"/>
     </row>
     <row r="26" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G26" s="29"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="31"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="32"/>
     </row>
     <row r="27" spans="7:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G27" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="H27" s="36"/>
-      <c r="I27" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="J27" s="37"/>
+      <c r="G27" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="37"/>
+      <c r="I27" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="38"/>
     </row>
     <row r="28" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G28" s="26"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="28"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G29" s="26"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="28"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="29"/>
     </row>
     <row r="30" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G30" s="26"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="28"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="29"/>
     </row>
     <row r="31" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G31" s="26"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="28"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="29"/>
     </row>
     <row r="32" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G32" s="26"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="28"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="29"/>
     </row>
     <row r="33" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G33" s="26"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="28"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="29"/>
     </row>
     <row r="34" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="29"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="31"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="32"/>
     </row>
     <row r="35" spans="7:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G35" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="37"/>
+      <c r="G35" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="38"/>
     </row>
     <row r="36" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G36" s="26"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="28"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="49"/>
     </row>
     <row r="37" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G37" s="26"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="28"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="49"/>
     </row>
     <row r="38" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G38" s="26"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="28"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="49"/>
     </row>
     <row r="39" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G39" s="26"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="28"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="49"/>
     </row>
     <row r="40" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G40" s="26"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="28"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="40"/>
+      <c r="I40" s="40"/>
+      <c r="J40" s="49"/>
     </row>
     <row r="41" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G41" s="26"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="28"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="40"/>
+      <c r="I41" s="40"/>
+      <c r="J41" s="49"/>
     </row>
     <row r="42" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G42" s="29"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="31"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="51"/>
+      <c r="I42" s="51"/>
+      <c r="J42" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="44">
@@ -1317,14 +1347,14 @@
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="I32:J32"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
     <mergeCell ref="G23:J23"/>
     <mergeCell ref="G15:J15"/>
     <mergeCell ref="G8:J8"/>
     <mergeCell ref="G26:J26"/>
     <mergeCell ref="H24:J24"/>
     <mergeCell ref="H25:J25"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="G17:H17"/>

</xml_diff>